<commit_message>
Add computation model for 2 states
</commit_message>
<xml_diff>
--- a/notebooks/ib_extended_essay/data/population-nst-est2020.xlsx
+++ b/notebooks/ib_extended_essay/data/population-nst-est2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10808"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Shared\ESTIMATES\V2020\Team Specific Material\Dissemination\Products\DISS\Products with April 1, 2020 Estimates\Table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akhilkarra/ode/python-lab/notebooks/ib_extended_essay/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8B1353-0EFE-4922-8B5C-713708396A13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A08425-F641-BB40-86CF-BD0298E627E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NST01" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,18 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'NST01'!$A$2:$O$68</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'NST01'!$A:$A,'NST01'!$2:$4</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -772,7 +783,7 @@
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1496,18 +1507,18 @@
   <dimension ref="A1:O68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:O2"/>
+      <selection activeCell="O53" sqref="O53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
     <col min="2" max="14" width="14.6640625" style="1" customWidth="1"/>
     <col min="15" max="15" width="13" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.109375" style="1"/>
+    <col min="16" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="2.25" customHeight="1">
       <c r="A1" s="23" t="s">
         <v>5</v>
       </c>
@@ -1526,7 +1537,7 @@
       <c r="N1" s="23"/>
       <c r="O1" s="23"/>
     </row>
-    <row r="2" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="25.5" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>70</v>
       </c>
@@ -1545,7 +1556,7 @@
       <c r="N2" s="25"/>
       <c r="O2" s="25"/>
     </row>
-    <row r="3" spans="1:15" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="10" customFormat="1" ht="14.5" customHeight="1">
       <c r="A3" s="26" t="s">
         <v>6</v>
       </c>
@@ -1570,7 +1581,7 @@
       </c>
       <c r="O3" s="37"/>
     </row>
-    <row r="4" spans="1:15" s="2" customFormat="1" ht="25.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" s="2" customFormat="1">
       <c r="A4" s="27"/>
       <c r="B4" s="13" t="s">
         <v>7</v>
@@ -1615,7 +1626,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1662,7 +1673,7 @@
         <v>329484123</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15">
       <c r="A6" s="5" t="s">
         <v>1</v>
       </c>
@@ -1709,7 +1720,7 @@
         <v>55849869</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15">
       <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
@@ -1756,7 +1767,7 @@
         <v>68316744</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -1803,7 +1814,7 @@
         <v>126662754</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15">
       <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
@@ -1850,7 +1861,7 @@
         <v>78654756</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15">
       <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
@@ -1897,7 +1908,7 @@
         <v>4921532</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -1944,7 +1955,7 @@
         <v>731158</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15">
       <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
@@ -1991,7 +2002,7 @@
         <v>7421401</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
@@ -2038,7 +2049,7 @@
         <v>3030522</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15">
       <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
@@ -2085,7 +2096,7 @@
         <v>39368078</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15">
       <c r="A15" s="9" t="s">
         <v>15</v>
       </c>
@@ -2132,7 +2143,7 @@
         <v>5807719</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15">
       <c r="A16" s="9" t="s">
         <v>16</v>
       </c>
@@ -2179,7 +2190,7 @@
         <v>3557006</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15">
       <c r="A17" s="9" t="s">
         <v>17</v>
       </c>
@@ -2226,7 +2237,7 @@
         <v>986809</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15">
       <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
@@ -2273,7 +2284,7 @@
         <v>712816</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15">
       <c r="A19" s="9" t="s">
         <v>19</v>
       </c>
@@ -2320,7 +2331,7 @@
         <v>21733312</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15">
       <c r="A20" s="9" t="s">
         <v>20</v>
       </c>
@@ -2367,7 +2378,7 @@
         <v>10710017</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15">
       <c r="A21" s="9" t="s">
         <v>21</v>
       </c>
@@ -2414,7 +2425,7 @@
         <v>1407006</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15">
       <c r="A22" s="9" t="s">
         <v>22</v>
       </c>
@@ -2461,7 +2472,7 @@
         <v>1826913</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15">
       <c r="A23" s="9" t="s">
         <v>23</v>
       </c>
@@ -2508,7 +2519,7 @@
         <v>12587530</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15">
       <c r="A24" s="9" t="s">
         <v>24</v>
       </c>
@@ -2555,7 +2566,7 @@
         <v>6754953</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15">
       <c r="A25" s="9" t="s">
         <v>25</v>
       </c>
@@ -2602,7 +2613,7 @@
         <v>3163561</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15">
       <c r="A26" s="9" t="s">
         <v>26</v>
       </c>
@@ -2649,7 +2660,7 @@
         <v>2913805</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15">
       <c r="A27" s="9" t="s">
         <v>27</v>
       </c>
@@ -2696,7 +2707,7 @@
         <v>4477251</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15">
       <c r="A28" s="9" t="s">
         <v>28</v>
       </c>
@@ -2743,7 +2754,7 @@
         <v>4645318</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15">
       <c r="A29" s="9" t="s">
         <v>29</v>
       </c>
@@ -2790,7 +2801,7 @@
         <v>1350141</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15">
       <c r="A30" s="9" t="s">
         <v>30</v>
       </c>
@@ -2837,7 +2848,7 @@
         <v>6055802</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15">
       <c r="A31" s="9" t="s">
         <v>31</v>
       </c>
@@ -2884,7 +2895,7 @@
         <v>6893574</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15">
       <c r="A32" s="9" t="s">
         <v>32</v>
       </c>
@@ -2931,7 +2942,7 @@
         <v>9966555</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15">
       <c r="A33" s="9" t="s">
         <v>33</v>
       </c>
@@ -2978,7 +2989,7 @@
         <v>5657342</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15">
       <c r="A34" s="9" t="s">
         <v>34</v>
       </c>
@@ -3025,7 +3036,7 @@
         <v>2966786</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15">
       <c r="A35" s="9" t="s">
         <v>35</v>
       </c>
@@ -3072,7 +3083,7 @@
         <v>6151548</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15">
       <c r="A36" s="9" t="s">
         <v>36</v>
       </c>
@@ -3119,7 +3130,7 @@
         <v>1080577</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15">
       <c r="A37" s="9" t="s">
         <v>37</v>
       </c>
@@ -3166,7 +3177,7 @@
         <v>1937552</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15">
       <c r="A38" s="9" t="s">
         <v>38</v>
       </c>
@@ -3213,7 +3224,7 @@
         <v>3138259</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15">
       <c r="A39" s="9" t="s">
         <v>39</v>
       </c>
@@ -3260,7 +3271,7 @@
         <v>1366275</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15">
       <c r="A40" s="9" t="s">
         <v>40</v>
       </c>
@@ -3307,7 +3318,7 @@
         <v>8882371</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15">
       <c r="A41" s="9" t="s">
         <v>41</v>
       </c>
@@ -3354,7 +3365,7 @@
         <v>2106319</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15">
       <c r="A42" s="9" t="s">
         <v>42</v>
       </c>
@@ -3401,7 +3412,7 @@
         <v>19336776</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15">
       <c r="A43" s="9" t="s">
         <v>43</v>
       </c>
@@ -3448,7 +3459,7 @@
         <v>10600823</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15">
       <c r="A44" s="9" t="s">
         <v>44</v>
       </c>
@@ -3495,7 +3506,7 @@
         <v>765309</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15">
       <c r="A45" s="9" t="s">
         <v>45</v>
       </c>
@@ -3542,7 +3553,7 @@
         <v>11693217</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15">
       <c r="A46" s="9" t="s">
         <v>46</v>
       </c>
@@ -3589,7 +3600,7 @@
         <v>3980783</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15">
       <c r="A47" s="9" t="s">
         <v>47</v>
       </c>
@@ -3636,7 +3647,7 @@
         <v>4241507</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15">
       <c r="A48" s="9" t="s">
         <v>48</v>
       </c>
@@ -3683,7 +3694,7 @@
         <v>12783254</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15">
       <c r="A49" s="9" t="s">
         <v>49</v>
       </c>
@@ -3730,7 +3741,7 @@
         <v>1057125</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15">
       <c r="A50" s="9" t="s">
         <v>50</v>
       </c>
@@ -3777,7 +3788,7 @@
         <v>5218040</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15">
       <c r="A51" s="9" t="s">
         <v>51</v>
       </c>
@@ -3824,7 +3835,7 @@
         <v>892717</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15">
       <c r="A52" s="9" t="s">
         <v>52</v>
       </c>
@@ -3871,7 +3882,7 @@
         <v>6886834</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15">
       <c r="A53" s="9" t="s">
         <v>53</v>
       </c>
@@ -3918,7 +3929,7 @@
         <v>29360759</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15">
       <c r="A54" s="9" t="s">
         <v>54</v>
       </c>
@@ -3965,7 +3976,7 @@
         <v>3249879</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15">
       <c r="A55" s="9" t="s">
         <v>55</v>
       </c>
@@ -4012,7 +4023,7 @@
         <v>623347</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15">
       <c r="A56" s="9" t="s">
         <v>56</v>
       </c>
@@ -4059,7 +4070,7 @@
         <v>8590563</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15">
       <c r="A57" s="9" t="s">
         <v>57</v>
       </c>
@@ -4106,7 +4117,7 @@
         <v>7693612</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15">
       <c r="A58" s="9" t="s">
         <v>58</v>
       </c>
@@ -4153,7 +4164,7 @@
         <v>1784787</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15">
       <c r="A59" s="9" t="s">
         <v>59</v>
       </c>
@@ -4200,7 +4211,7 @@
         <v>5832655</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15">
       <c r="A60" s="9" t="s">
         <v>60</v>
       </c>
@@ -4247,7 +4258,7 @@
         <v>582328</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15">
       <c r="A61" s="9"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -4264,7 +4275,7 @@
       <c r="N61" s="6"/>
       <c r="O61" s="6"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15">
       <c r="A62" s="11" t="s">
         <v>63</v>
       </c>
@@ -4311,7 +4322,7 @@
         <v>3159343</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" ht="51" customHeight="1">
       <c r="A63" s="30" t="s">
         <v>67</v>
       </c>
@@ -4330,7 +4341,7 @@
       <c r="N63" s="31"/>
       <c r="O63" s="32"/>
     </row>
-    <row r="64" spans="1:15" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" ht="20.5" customHeight="1">
       <c r="A64" s="30" t="s">
         <v>68</v>
       </c>
@@ -4349,7 +4360,7 @@
       <c r="N64" s="31"/>
       <c r="O64" s="32"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15">
       <c r="A65" s="14" t="s">
         <v>61</v>
       </c>
@@ -4368,7 +4379,7 @@
       <c r="N65" s="15"/>
       <c r="O65" s="16"/>
     </row>
-    <row r="66" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" ht="12.75" customHeight="1">
       <c r="A66" s="17" t="s">
         <v>71</v>
       </c>
@@ -4387,7 +4398,7 @@
       <c r="N66" s="18"/>
       <c r="O66" s="19"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15">
       <c r="A67" s="17" t="s">
         <v>62</v>
       </c>
@@ -4406,7 +4417,7 @@
       <c r="N67" s="18"/>
       <c r="O67" s="19"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15">
       <c r="A68" s="20" t="s">
         <v>69</v>
       </c>

</xml_diff>